<commit_message>
updated code and added CIMIS data
</commit_message>
<xml_diff>
--- a/Precipitation/hourly/hourly_stations_list.xlsx
+++ b/Precipitation/hourly/hourly_stations_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>CA047772</t>
   </si>
@@ -96,6 +96,72 @@
   </si>
   <si>
     <t>Saint Helena</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>SF Bay Reserve</t>
+  </si>
+  <si>
+    <t>Downtown</t>
+  </si>
+  <si>
+    <t>Peraluma Municipal Airport</t>
+  </si>
+  <si>
+    <t>SJC</t>
+  </si>
+  <si>
+    <t>SFO</t>
+  </si>
+  <si>
+    <t>Sonoma County Airport</t>
+  </si>
+  <si>
+    <t>WBAN:23272</t>
+  </si>
+  <si>
+    <t>WBAN:99999</t>
+  </si>
+  <si>
+    <t>WBAN:23285</t>
+  </si>
+  <si>
+    <t>WBAN:00320</t>
+  </si>
+  <si>
+    <t>WBAN:23293</t>
+  </si>
+  <si>
+    <t>WBAN:23234</t>
+  </si>
+  <si>
+    <t>WBAN:23213</t>
+  </si>
+  <si>
+    <t>Half Moon Bay Airport</t>
+  </si>
+  <si>
+    <t>WBAN:00228</t>
+  </si>
+  <si>
+    <t>Reid-Hillview Airport of Sana Clara</t>
+  </si>
+  <si>
+    <t>WBAN:93232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palo Alto Airport </t>
+  </si>
+  <si>
+    <t>WBAN:23289</t>
+  </si>
+  <si>
+    <t>San Carlos Airport</t>
+  </si>
+  <si>
+    <t>WBAN:93231</t>
   </si>
 </sst>
 </file>
@@ -413,112 +479,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>